<commit_message>
db structure changed, foreign key added
</commit_message>
<xml_diff>
--- a/Info projet/Journal de bord.xlsx
+++ b/Info projet/Journal de bord.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\php\CoiffureKopp\Info projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{794F0B3F-3870-40D9-B17F-00C98E0F7B9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA0C1B4-26CB-4A21-949F-82BCE6998882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{F8502FEA-3956-43AF-B55B-B0944DFFB583}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="20">
   <si>
     <t>Date</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Scooting &amp; recherche d'idées (templates etc..)</t>
   </si>
   <si>
-    <t>HTML</t>
-  </si>
-  <si>
     <t>Création de structure MVC + configuration BDD</t>
   </si>
   <si>
@@ -69,6 +66,36 @@
   </si>
   <si>
     <t>CRUD Admin</t>
+  </si>
+  <si>
+    <t>CRUD Content</t>
+  </si>
+  <si>
+    <t>FRONT Barre nav, structure de page</t>
+  </si>
+  <si>
+    <t>FRONT Footer, Charte graphique</t>
+  </si>
+  <si>
+    <t>HTML + PHP</t>
+  </si>
+  <si>
+    <t>HTML + PHP + MySQL</t>
+  </si>
+  <si>
+    <t>HTML + JS + CSS</t>
+  </si>
+  <si>
+    <t>HTML + JS + CSS + PHP</t>
+  </si>
+  <si>
+    <t>FRONT Page Actualité (Dynamique)</t>
+  </si>
+  <si>
+    <t>FRONT Page Equipe (Statique)</t>
+  </si>
+  <si>
+    <t>FRONT Page Salon  (Dynamique)</t>
   </si>
 </sst>
 </file>
@@ -424,7 +451,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,13 +495,13 @@
         <v>45048</v>
       </c>
       <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -482,104 +509,167 @@
         <v>45049</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45050</v>
       </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
       <c r="C5" t="s">
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45051</v>
       </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
       <c r="C6" t="s">
         <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45052</v>
       </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
       <c r="C7" t="s">
         <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>45053</v>
       </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
       <c r="C8" t="s">
         <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>45054</v>
       </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
       <c r="C9" t="s">
         <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>45055</v>
       </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
       <c r="C10" t="s">
         <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>45056</v>
       </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
       <c r="C11" t="s">
         <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>45057</v>
       </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
       <c r="C12" t="s">
         <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>45058</v>
       </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
       <c r="C13" t="s">
         <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>45059</v>
       </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
       <c r="C14" t="s">
         <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>45060</v>
       </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
       <c r="C15" t="s">
         <v>5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>